<commit_message>
Updated function point calculation
</commit_message>
<xml_diff>
--- a/Function Points.xlsx
+++ b/Function Points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mails\Documents\GitHub\ikindo-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E312D38D-3F3C-4723-AAFE-83D97C896A74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36438AD0-2423-4A38-A66C-5786C7123416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{BF893BD0-8458-4AAA-9564-FE13012D0CBA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>View Site</t>
   </si>
@@ -74,12 +74,15 @@
   <si>
     <t>FP (Old)</t>
   </si>
+  <si>
+    <t>Real Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +98,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,14 +128,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -232,10 +250,10 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="l"/>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -380,7 +398,7 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="l"/>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -463,8 +481,105 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Real Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="10"/>
+            <c:backward val="5"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.705882352941176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.617647058823529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.970588235294118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0542-4FF3-AB49-F9E8BBA6B0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
-          <c:dLblPos val="l"/>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1352,15 +1467,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1685,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D361C2FD-2695-4EAF-9160-48408FC633FE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1813,7 @@
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1709,7 +1824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1835,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1846,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1741,20 +1856,26 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f>C5/0.884</f>
         <v>22.058823529411764</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>19.5</v>
       </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1765,8 +1886,11 @@
       <c r="C6">
         <v>11.05</v>
       </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1777,8 +1901,11 @@
       <c r="C7">
         <v>13</v>
       </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1789,8 +1916,11 @@
       <c r="C8">
         <v>27.95</v>
       </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1800,6 +1930,9 @@
       </c>
       <c r="C9">
         <v>12.35</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>